<commit_message>
start of writing to xlsx
</commit_message>
<xml_diff>
--- a/test_in.xlsx
+++ b/test_in.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr updateLinks="always" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\PycharmProjects\mvl_gui\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="WE 07-05-10" sheetId="2" r:id="rId1"/>
@@ -3056,8 +3056,8 @@
       <sheetName val="WE 09-20-13"/>
       <sheetName val="WE 09-13-13"/>
       <sheetName val="WE 09-06-13"/>
+      <sheetName val="WE 12-14-12"/>
       <sheetName val="WE 12-14-12 (2)"/>
-      <sheetName val="WE 12-14-12"/>
       <sheetName val="WE 12-07-12"/>
       <sheetName val="WE 11-29-12"/>
       <sheetName val="WE 11-22-12"/>
@@ -3143,6 +3143,7 @@
       <sheetName val="WE 05-15-11"/>
       <sheetName val="WE 05-08-11"/>
       <sheetName val="WE 05-01-11"/>
+      <sheetName val="WE 04-24-11"/>
       <sheetName val="WE 04-17-11"/>
       <sheetName val="WE 04-10-11"/>
       <sheetName val="WE 04-03-11"/>
@@ -3411,14 +3412,14 @@
       <sheetData sheetId="194"/>
       <sheetData sheetId="195"/>
       <sheetData sheetId="196"/>
-      <sheetData sheetId="197">
+      <sheetData sheetId="197"/>
+      <sheetData sheetId="198">
         <row r="9">
           <cell r="B9">
             <v>30000</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="198"/>
       <sheetData sheetId="199"/>
       <sheetData sheetId="200"/>
       <sheetData sheetId="201"/>
@@ -3474,6 +3475,7 @@
       <sheetData sheetId="251"/>
       <sheetData sheetId="252"/>
       <sheetData sheetId="253"/>
+      <sheetData sheetId="254"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -3781,7 +3783,7 @@
   </sheetPr>
   <dimension ref="A1:AF148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="H36" sqref="H36:I37"/>
     </sheetView>
   </sheetViews>
@@ -22029,7 +22031,7 @@
   <dimension ref="A1:AI148"/>
   <sheetViews>
     <sheetView zoomScale="75" workbookViewId="0">
-      <selection activeCell="S114" sqref="S114:S117"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -31341,7 +31343,7 @@
   <dimension ref="A1:AD148"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="I37" sqref="H33:I37"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -40152,8 +40154,8 @@
   </sheetPr>
   <dimension ref="A1:AD148"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -40192,7 +40194,7 @@
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" s="1">
-        <f>+B1</f>
+        <f>B1</f>
         <v>42490</v>
       </c>
       <c r="B1" s="372">
@@ -40209,10 +40211,10 @@
     </row>
     <row r="2" spans="1:30" ht="13.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <f>+B2</f>
+        <f>B2</f>
         <v>42496</v>
       </c>
-      <c r="B2" s="373">
+      <c r="B2" s="374">
         <v>42496</v>
       </c>
       <c r="C2" s="4" t="s">

</xml_diff>